<commit_message>
Modeled the health of the UT rice data
</commit_message>
<xml_diff>
--- a/UT_Rice_2022/2022-09-25_AS7265x_dead.xlsx
+++ b/UT_Rice_2022/2022-09-25_AS7265x_dead.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\วิทยานิพนธ์\ปริมาณคลอโรฟิลล์ใบที่ตาย\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zanith\PycharmProjects\sklearn_scripts\UT_Rice_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB15FDB-7224-4951-B890-2DE7E63DFE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A27BB-3CD1-4660-B2C9-00F497310ABB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{473BACF8-5717-4BDB-BB50-0E41476D7781}"/>
   </bookViews>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -119,15 +111,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>หมายเลขกระถาง</t>
-  </si>
-  <si>
-    <t>การทดลอง</t>
-  </si>
-  <si>
-    <t>พันธุ์</t>
-  </si>
-  <si>
     <t>กระดาษขาว</t>
   </si>
   <si>
@@ -145,16 +128,25 @@
   <si>
     <t>ปทุมธษนี 1</t>
   </si>
+  <si>
+    <t>variety</t>
+  </si>
+  <si>
+    <t>pot number</t>
+  </si>
+  <si>
+    <t>type exp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -185,7 +177,7 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,7 +193,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,21 +491,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64957E9-8008-4E33-8AE3-BA832F8459F2}">
   <dimension ref="A1:AC405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -594,9 +586,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29">
       <c r="C2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -674,7 +666,7 @@
         <v>0.6999305555555555</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29">
       <c r="D3">
         <v>1</v>
       </c>
@@ -751,7 +743,7 @@
         <v>0.69995370370370369</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29">
       <c r="D4">
         <v>1</v>
       </c>
@@ -828,7 +820,7 @@
         <v>0.69997685185185177</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29">
       <c r="D5">
         <v>1</v>
       </c>
@@ -905,15 +897,15 @@
         <v>0.70001157407407411</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -991,7 +983,7 @@
         <v>0.70105324074074071</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29">
       <c r="D7">
         <v>2</v>
       </c>
@@ -1068,7 +1060,7 @@
         <v>0.70108796296296294</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29">
       <c r="D8">
         <v>2</v>
       </c>
@@ -1145,7 +1137,7 @@
         <v>0.70111111111111113</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29">
       <c r="D9">
         <v>2</v>
       </c>
@@ -1222,9 +1214,9 @@
         <v>0.70113425925925921</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29">
       <c r="C10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1302,7 +1294,7 @@
         <v>0.70170138888888889</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29">
       <c r="D11">
         <v>3</v>
       </c>
@@ -1379,7 +1371,7 @@
         <v>0.70173611111111101</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29">
       <c r="D12">
         <v>3</v>
       </c>
@@ -1456,7 +1448,7 @@
         <v>0.7017592592592593</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29">
       <c r="D13">
         <v>3</v>
       </c>
@@ -1533,9 +1525,9 @@
         <v>0.70179398148148142</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29">
       <c r="C14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1613,7 +1605,7 @@
         <v>0.70216435185185189</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29">
       <c r="D15">
         <v>4</v>
       </c>
@@ -1690,7 +1682,7 @@
         <v>0.70219907407407411</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29">
       <c r="D16">
         <v>4</v>
       </c>
@@ -1767,7 +1759,7 @@
         <v>0.70222222222222219</v>
       </c>
     </row>
-    <row r="17" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:28">
       <c r="D17">
         <v>4</v>
       </c>
@@ -1844,9 +1836,9 @@
         <v>0.70225694444444453</v>
       </c>
     </row>
-    <row r="18" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:28">
       <c r="C18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -1924,7 +1916,7 @@
         <v>0.70281249999999995</v>
       </c>
     </row>
-    <row r="19" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:28">
       <c r="D19">
         <v>5</v>
       </c>
@@ -2001,7 +1993,7 @@
         <v>0.70283564814814825</v>
       </c>
     </row>
-    <row r="20" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:28">
       <c r="D20">
         <v>5</v>
       </c>
@@ -2078,7 +2070,7 @@
         <v>0.70287037037037037</v>
       </c>
     </row>
-    <row r="21" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:28">
       <c r="D21">
         <v>5</v>
       </c>
@@ -2155,9 +2147,9 @@
         <v>0.7029050925925926</v>
       </c>
     </row>
-    <row r="22" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:28">
       <c r="C22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -2235,7 +2227,7 @@
         <v>0.70332175925925933</v>
       </c>
     </row>
-    <row r="23" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:28">
       <c r="D23">
         <v>6</v>
       </c>
@@ -2312,7 +2304,7 @@
         <v>0.7033449074074074</v>
       </c>
     </row>
-    <row r="24" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:28">
       <c r="D24">
         <v>6</v>
       </c>
@@ -2389,7 +2381,7 @@
         <v>0.70337962962962963</v>
       </c>
     </row>
-    <row r="25" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:28">
       <c r="D25">
         <v>6</v>
       </c>
@@ -2466,9 +2458,9 @@
         <v>0.70340277777777782</v>
       </c>
     </row>
-    <row r="26" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:28">
       <c r="C26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D26">
         <v>7</v>
@@ -2546,7 +2538,7 @@
         <v>0.70535879629629628</v>
       </c>
     </row>
-    <row r="27" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:28">
       <c r="D27">
         <v>7</v>
       </c>
@@ -2623,7 +2615,7 @@
         <v>0.70539351851851861</v>
       </c>
     </row>
-    <row r="28" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:28">
       <c r="D28">
         <v>7</v>
       </c>
@@ -2700,7 +2692,7 @@
         <v>0.70541666666666669</v>
       </c>
     </row>
-    <row r="29" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:28">
       <c r="D29">
         <v>7</v>
       </c>
@@ -2777,9 +2769,9 @@
         <v>0.70545138888888881</v>
       </c>
     </row>
-    <row r="30" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:28">
       <c r="C30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D30">
         <v>8</v>
@@ -2857,7 +2849,7 @@
         <v>0.70594907407407403</v>
       </c>
     </row>
-    <row r="31" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:28">
       <c r="D31">
         <v>8</v>
       </c>
@@ -2934,7 +2926,7 @@
         <v>0.70597222222222233</v>
       </c>
     </row>
-    <row r="32" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:28">
       <c r="D32">
         <v>8</v>
       </c>
@@ -3011,7 +3003,7 @@
         <v>0.70600694444444445</v>
       </c>
     </row>
-    <row r="33" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:28">
       <c r="D33">
         <v>8</v>
       </c>
@@ -3088,9 +3080,9 @@
         <v>0.70604166666666668</v>
       </c>
     </row>
-    <row r="34" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:28">
       <c r="C34" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D34">
         <v>9</v>
@@ -3168,7 +3160,7 @@
         <v>0.70636574074074077</v>
       </c>
     </row>
-    <row r="35" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:28">
       <c r="D35">
         <v>9</v>
       </c>
@@ -3245,7 +3237,7 @@
         <v>0.70640046296296299</v>
       </c>
     </row>
-    <row r="36" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:28">
       <c r="D36">
         <v>9</v>
       </c>
@@ -3322,7 +3314,7 @@
         <v>0.70643518518518522</v>
       </c>
     </row>
-    <row r="37" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:28">
       <c r="D37">
         <v>9</v>
       </c>
@@ -3399,9 +3391,9 @@
         <v>0.70646990740740734</v>
       </c>
     </row>
-    <row r="38" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:28">
       <c r="C38" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D38">
         <v>10</v>
@@ -3479,7 +3471,7 @@
         <v>0.70699074074074064</v>
       </c>
     </row>
-    <row r="39" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:28">
       <c r="D39">
         <v>10</v>
       </c>
@@ -3556,7 +3548,7 @@
         <v>0.70701388888888894</v>
       </c>
     </row>
-    <row r="40" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:28">
       <c r="D40">
         <v>10</v>
       </c>
@@ -3633,7 +3625,7 @@
         <v>0.70704861111111106</v>
       </c>
     </row>
-    <row r="41" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:28">
       <c r="D41">
         <v>10</v>
       </c>
@@ -3710,9 +3702,9 @@
         <v>0.70707175925925936</v>
       </c>
     </row>
-    <row r="42" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:28">
       <c r="C42" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D42">
         <v>11</v>
@@ -3790,7 +3782,7 @@
         <v>0.70843750000000005</v>
       </c>
     </row>
-    <row r="43" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:28">
       <c r="D43">
         <v>11</v>
       </c>
@@ -3867,7 +3859,7 @@
         <v>0.70847222222222228</v>
       </c>
     </row>
-    <row r="44" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:28">
       <c r="D44">
         <v>11</v>
       </c>
@@ -3944,7 +3936,7 @@
         <v>0.70849537037037036</v>
       </c>
     </row>
-    <row r="45" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:28">
       <c r="D45">
         <v>11</v>
       </c>
@@ -4021,9 +4013,9 @@
         <v>0.7085300925925927</v>
       </c>
     </row>
-    <row r="46" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:28">
       <c r="C46" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D46">
         <v>12</v>
@@ -4101,7 +4093,7 @@
         <v>0.70896990740740751</v>
       </c>
     </row>
-    <row r="47" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:28">
       <c r="D47">
         <v>12</v>
       </c>
@@ -4178,7 +4170,7 @@
         <v>0.70900462962962962</v>
       </c>
     </row>
-    <row r="48" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:28">
       <c r="D48">
         <v>12</v>
       </c>
@@ -4255,7 +4247,7 @@
         <v>0.7090277777777777</v>
       </c>
     </row>
-    <row r="49" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:28">
       <c r="D49">
         <v>12</v>
       </c>
@@ -4332,9 +4324,9 @@
         <v>0.70906249999999993</v>
       </c>
     </row>
-    <row r="50" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:28">
       <c r="C50" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D50">
         <v>13</v>
@@ -4412,7 +4404,7 @@
         <v>0.70940972222222232</v>
       </c>
     </row>
-    <row r="51" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:28">
       <c r="D51">
         <v>13</v>
       </c>
@@ -4489,7 +4481,7 @@
         <v>0.70943287037037039</v>
       </c>
     </row>
-    <row r="52" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:28">
       <c r="D52">
         <v>13</v>
       </c>
@@ -4566,7 +4558,7 @@
         <v>0.70946759259259251</v>
       </c>
     </row>
-    <row r="53" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:28">
       <c r="D53">
         <v>13</v>
       </c>
@@ -4643,9 +4635,9 @@
         <v>0.70950231481481485</v>
       </c>
     </row>
-    <row r="54" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:28">
       <c r="C54" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D54">
         <v>14</v>
@@ -4723,7 +4715,7 @@
         <v>0.71015046296296302</v>
       </c>
     </row>
-    <row r="55" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:28">
       <c r="D55">
         <v>14</v>
       </c>
@@ -4800,7 +4792,7 @@
         <v>0.7101736111111111</v>
       </c>
     </row>
-    <row r="56" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:28">
       <c r="D56">
         <v>14</v>
       </c>
@@ -4877,7 +4869,7 @@
         <v>0.71020833333333344</v>
       </c>
     </row>
-    <row r="57" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:28">
       <c r="D57">
         <v>14</v>
       </c>
@@ -4954,9 +4946,9 @@
         <v>0.71023148148148152</v>
       </c>
     </row>
-    <row r="58" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:28">
       <c r="C58" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D58">
         <v>15</v>
@@ -5034,7 +5026,7 @@
         <v>0.7106365740740741</v>
       </c>
     </row>
-    <row r="59" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:28">
       <c r="D59">
         <v>15</v>
       </c>
@@ -5111,7 +5103,7 @@
         <v>0.71067129629629633</v>
       </c>
     </row>
-    <row r="60" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:28">
       <c r="D60">
         <v>15</v>
       </c>
@@ -5188,7 +5180,7 @@
         <v>0.71070601851851845</v>
       </c>
     </row>
-    <row r="61" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:28">
       <c r="D61">
         <v>15</v>
       </c>
@@ -5265,9 +5257,9 @@
         <v>0.71074074074074067</v>
       </c>
     </row>
-    <row r="62" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:28">
       <c r="C62" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D62">
         <v>16</v>
@@ -5345,7 +5337,7 @@
         <v>0.71116898148148155</v>
       </c>
     </row>
-    <row r="63" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:28">
       <c r="D63">
         <v>16</v>
       </c>
@@ -5422,7 +5414,7 @@
         <v>0.71120370370370367</v>
       </c>
     </row>
-    <row r="64" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:28">
       <c r="D64">
         <v>16</v>
       </c>
@@ -5499,7 +5491,7 @@
         <v>0.7112384259259259</v>
       </c>
     </row>
-    <row r="65" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:28">
       <c r="D65">
         <v>16</v>
       </c>
@@ -5576,9 +5568,9 @@
         <v>0.71126157407407409</v>
       </c>
     </row>
-    <row r="66" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:28">
       <c r="C66" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D66">
         <v>17</v>
@@ -5656,7 +5648,7 @@
         <v>0.71240740740740749</v>
       </c>
     </row>
-    <row r="67" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:28">
       <c r="D67">
         <v>17</v>
       </c>
@@ -5733,7 +5725,7 @@
         <v>0.71244212962962961</v>
       </c>
     </row>
-    <row r="68" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:28">
       <c r="D68">
         <v>17</v>
       </c>
@@ -5810,7 +5802,7 @@
         <v>0.71247685185185183</v>
       </c>
     </row>
-    <row r="69" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:28">
       <c r="D69">
         <v>17</v>
       </c>
@@ -5887,9 +5879,9 @@
         <v>0.71251157407407406</v>
       </c>
     </row>
-    <row r="70" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:28">
       <c r="C70" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D70">
         <v>18</v>
@@ -5967,7 +5959,7 @@
         <v>0.71288194444444442</v>
       </c>
     </row>
-    <row r="71" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:28">
       <c r="D71">
         <v>18</v>
       </c>
@@ -6044,7 +6036,7 @@
         <v>0.71290509259259249</v>
       </c>
     </row>
-    <row r="72" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:28">
       <c r="D72">
         <v>18</v>
       </c>
@@ -6121,7 +6113,7 @@
         <v>0.71293981481481483</v>
       </c>
     </row>
-    <row r="73" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:28">
       <c r="D73">
         <v>18</v>
       </c>
@@ -6198,9 +6190,9 @@
         <v>0.71298611111111121</v>
       </c>
     </row>
-    <row r="74" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:28">
       <c r="C74" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D74">
         <v>19</v>
@@ -6278,7 +6270,7 @@
         <v>0.71369212962962969</v>
       </c>
     </row>
-    <row r="75" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:28">
       <c r="D75">
         <v>19</v>
       </c>
@@ -6355,7 +6347,7 @@
         <v>0.71372685185185192</v>
       </c>
     </row>
-    <row r="76" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:28">
       <c r="D76">
         <v>19</v>
       </c>
@@ -6432,7 +6424,7 @@
         <v>0.71376157407407403</v>
       </c>
     </row>
-    <row r="77" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:28">
       <c r="D77">
         <v>19</v>
       </c>
@@ -6509,9 +6501,9 @@
         <v>0.71378472222222211</v>
       </c>
     </row>
-    <row r="78" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:28">
       <c r="C78" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D78">
         <v>20</v>
@@ -6589,7 +6581,7 @@
         <v>0.71432870370370372</v>
       </c>
     </row>
-    <row r="79" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:28">
       <c r="D79">
         <v>20</v>
       </c>
@@ -6666,7 +6658,7 @@
         <v>0.71436342592592583</v>
       </c>
     </row>
-    <row r="80" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:28">
       <c r="D80">
         <v>20</v>
       </c>
@@ -6743,7 +6735,7 @@
         <v>0.71439814814814817</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28">
       <c r="D81">
         <v>20</v>
       </c>
@@ -6820,9 +6812,9 @@
         <v>0.71442129629629625</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28">
       <c r="C82" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D82">
         <v>21</v>
@@ -6900,7 +6892,7 @@
         <v>0.71508101851851846</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28">
       <c r="D83">
         <v>21</v>
       </c>
@@ -6977,7 +6969,7 @@
         <v>0.71510416666666676</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28">
       <c r="D84">
         <v>21</v>
       </c>
@@ -7054,7 +7046,7 @@
         <v>0.71513888888888888</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28">
       <c r="D85">
         <v>21</v>
       </c>
@@ -7131,15 +7123,15 @@
         <v>0.71517361111111111</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28">
       <c r="A86">
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D86">
         <v>22</v>
@@ -7217,7 +7209,7 @@
         <v>0.71582175925925917</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28">
       <c r="D87">
         <v>22</v>
       </c>
@@ -7294,7 +7286,7 @@
         <v>0.71584490740740747</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28">
       <c r="D88">
         <v>22</v>
       </c>
@@ -7371,7 +7363,7 @@
         <v>0.71586805555555555</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28">
       <c r="D89">
         <v>22</v>
       </c>
@@ -7448,9 +7440,9 @@
         <v>0.71589120370370374</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28">
       <c r="C90" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D90">
         <v>23</v>
@@ -7528,7 +7520,7 @@
         <v>0.7166435185185186</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28">
       <c r="D91">
         <v>23</v>
       </c>
@@ -7605,7 +7597,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28">
       <c r="D92">
         <v>23</v>
       </c>
@@ -7682,7 +7674,7 @@
         <v>0.71668981481481486</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28">
       <c r="D93">
         <v>23</v>
       </c>
@@ -7759,9 +7751,9 @@
         <v>0.71672453703703709</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28">
       <c r="C94" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D94">
         <v>24</v>
@@ -7839,7 +7831,7 @@
         <v>0.71712962962962967</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28">
       <c r="D95">
         <v>24</v>
       </c>
@@ -7916,7 +7908,7 @@
         <v>0.71717592592592594</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28">
       <c r="D96">
         <v>24</v>
       </c>
@@ -7993,7 +7985,7 @@
         <v>0.71721064814814817</v>
       </c>
     </row>
-    <row r="97" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:28">
       <c r="D97">
         <v>24</v>
       </c>
@@ -8070,9 +8062,9 @@
         <v>0.71724537037037039</v>
       </c>
     </row>
-    <row r="98" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:28">
       <c r="C98" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D98">
         <v>25</v>
@@ -8150,7 +8142,7 @@
         <v>0.71763888888888883</v>
       </c>
     </row>
-    <row r="99" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:28">
       <c r="D99">
         <v>25</v>
       </c>
@@ -8227,7 +8219,7 @@
         <v>0.71765046296296298</v>
       </c>
     </row>
-    <row r="100" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:28">
       <c r="D100">
         <v>25</v>
       </c>
@@ -8304,7 +8296,7 @@
         <v>0.71767361111111105</v>
       </c>
     </row>
-    <row r="101" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:28">
       <c r="D101">
         <v>25</v>
       </c>
@@ -8381,9 +8373,9 @@
         <v>0.71770833333333339</v>
       </c>
     </row>
-    <row r="102" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:28">
       <c r="C102" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D102">
         <v>26</v>
@@ -8461,7 +8453,7 @@
         <v>0.71821759259259255</v>
       </c>
     </row>
-    <row r="103" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:28">
       <c r="D103">
         <v>26</v>
       </c>
@@ -8538,7 +8530,7 @@
         <v>0.71824074074074085</v>
       </c>
     </row>
-    <row r="104" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:28">
       <c r="D104">
         <v>26</v>
       </c>
@@ -8615,7 +8607,7 @@
         <v>0.71827546296296296</v>
       </c>
     </row>
-    <row r="105" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:28">
       <c r="D105">
         <v>26</v>
       </c>
@@ -8692,9 +8684,9 @@
         <v>0.71829861111111104</v>
       </c>
     </row>
-    <row r="106" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:28">
       <c r="C106" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D106">
         <v>27</v>
@@ -8772,7 +8764,7 @@
         <v>0.7193518518518518</v>
       </c>
     </row>
-    <row r="107" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:28">
       <c r="D107">
         <v>27</v>
       </c>
@@ -8849,7 +8841,7 @@
         <v>0.71937499999999999</v>
       </c>
     </row>
-    <row r="108" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:28">
       <c r="D108">
         <v>27</v>
       </c>
@@ -8926,7 +8918,7 @@
         <v>0.71940972222222221</v>
       </c>
     </row>
-    <row r="109" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:28">
       <c r="D109">
         <v>27</v>
       </c>
@@ -9003,9 +8995,9 @@
         <v>0.71944444444444444</v>
       </c>
     </row>
-    <row r="110" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:28">
       <c r="C110" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D110">
         <v>28</v>
@@ -9083,7 +9075,7 @@
         <v>0.71969907407407396</v>
       </c>
     </row>
-    <row r="111" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:28">
       <c r="D111">
         <v>28</v>
       </c>
@@ -9160,7 +9152,7 @@
         <v>0.71974537037037034</v>
       </c>
     </row>
-    <row r="112" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:28">
       <c r="D112">
         <v>28</v>
       </c>
@@ -9237,7 +9229,7 @@
         <v>0.71976851851851853</v>
       </c>
     </row>
-    <row r="113" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:28">
       <c r="D113">
         <v>28</v>
       </c>
@@ -9314,9 +9306,9 @@
         <v>0.7198148148148148</v>
       </c>
     </row>
-    <row r="114" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:28">
       <c r="C114" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D114">
         <v>29</v>
@@ -9394,7 +9386,7 @@
         <v>0.72037037037037033</v>
       </c>
     </row>
-    <row r="115" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:28">
       <c r="D115">
         <v>29</v>
       </c>
@@ -9471,7 +9463,7 @@
         <v>0.72039351851851852</v>
       </c>
     </row>
-    <row r="116" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:28">
       <c r="D116">
         <v>29</v>
       </c>
@@ -9548,7 +9540,7 @@
         <v>0.72042824074074074</v>
       </c>
     </row>
-    <row r="117" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:28">
       <c r="D117">
         <v>29</v>
       </c>
@@ -9625,9 +9617,9 @@
         <v>0.72046296296296297</v>
       </c>
     </row>
-    <row r="118" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:28">
       <c r="C118" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D118">
         <v>30</v>
@@ -9705,7 +9697,7 @@
         <v>0.72082175925925929</v>
       </c>
     </row>
-    <row r="119" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:28">
       <c r="D119">
         <v>30</v>
       </c>
@@ -9782,7 +9774,7 @@
         <v>0.7208564814814814</v>
       </c>
     </row>
-    <row r="120" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:28">
       <c r="D120">
         <v>30</v>
       </c>
@@ -9859,7 +9851,7 @@
         <v>0.7208796296296297</v>
       </c>
     </row>
-    <row r="121" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:28">
       <c r="D121">
         <v>30</v>
       </c>
@@ -9936,9 +9928,9 @@
         <v>0.72090277777777778</v>
       </c>
     </row>
-    <row r="122" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:28">
       <c r="C122" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D122">
         <v>31</v>
@@ -10016,7 +10008,7 @@
         <v>0.72130787037037036</v>
       </c>
     </row>
-    <row r="123" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:28">
       <c r="D123">
         <v>31</v>
       </c>
@@ -10093,7 +10085,7 @@
         <v>0.72133101851851855</v>
       </c>
     </row>
-    <row r="124" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:28">
       <c r="D124">
         <v>31</v>
       </c>
@@ -10170,7 +10162,7 @@
         <v>0.72136574074074078</v>
       </c>
     </row>
-    <row r="125" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:28">
       <c r="D125">
         <v>31</v>
       </c>
@@ -10247,9 +10239,9 @@
         <v>0.72138888888888886</v>
       </c>
     </row>
-    <row r="126" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:28">
       <c r="C126" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D126">
         <v>32</v>
@@ -10327,7 +10319,7 @@
         <v>0.72228009259259263</v>
       </c>
     </row>
-    <row r="127" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:28">
       <c r="D127">
         <v>32</v>
       </c>
@@ -10404,7 +10396,7 @@
         <v>0.7223032407407407</v>
       </c>
     </row>
-    <row r="128" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:28">
       <c r="D128">
         <v>32</v>
       </c>
@@ -10481,7 +10473,7 @@
         <v>0.72232638888888889</v>
       </c>
     </row>
-    <row r="129" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:28">
       <c r="D129">
         <v>32</v>
       </c>
@@ -10558,9 +10550,9 @@
         <v>0.72236111111111112</v>
       </c>
     </row>
-    <row r="130" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:28">
       <c r="C130" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D130">
         <v>33</v>
@@ -10638,7 +10630,7 @@
         <v>0.72295138888888888</v>
       </c>
     </row>
-    <row r="131" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:28">
       <c r="D131">
         <v>33</v>
       </c>
@@ -10715,7 +10707,7 @@
         <v>0.72298611111111111</v>
       </c>
     </row>
-    <row r="132" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:28">
       <c r="D132">
         <v>33</v>
       </c>
@@ -10792,7 +10784,7 @@
         <v>0.72302083333333333</v>
       </c>
     </row>
-    <row r="133" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:28">
       <c r="D133">
         <v>33</v>
       </c>
@@ -10869,9 +10861,9 @@
         <v>0.72303240740740737</v>
       </c>
     </row>
-    <row r="134" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:28">
       <c r="C134" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D134">
         <v>34</v>
@@ -10949,7 +10941,7 @@
         <v>0.72439814814814818</v>
       </c>
     </row>
-    <row r="135" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:28">
       <c r="D135">
         <v>34</v>
       </c>
@@ -11026,7 +11018,7 @@
         <v>0.7244328703703703</v>
       </c>
     </row>
-    <row r="136" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:28">
       <c r="D136">
         <v>34</v>
       </c>
@@ -11103,7 +11095,7 @@
         <v>0.72446759259259252</v>
       </c>
     </row>
-    <row r="137" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:28">
       <c r="D137">
         <v>34</v>
       </c>
@@ -11180,9 +11172,9 @@
         <v>0.72450231481481486</v>
       </c>
     </row>
-    <row r="138" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:28">
       <c r="C138" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D138">
         <v>35</v>
@@ -11260,7 +11252,7 @@
         <v>0.7249768518518519</v>
       </c>
     </row>
-    <row r="139" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:28">
       <c r="D139">
         <v>35</v>
       </c>
@@ -11337,7 +11329,7 @@
         <v>0.72501157407407402</v>
       </c>
     </row>
-    <row r="140" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:28">
       <c r="D140">
         <v>35</v>
       </c>
@@ -11414,7 +11406,7 @@
         <v>0.72503472222222232</v>
       </c>
     </row>
-    <row r="141" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:28">
       <c r="D141">
         <v>35</v>
       </c>
@@ -11491,9 +11483,9 @@
         <v>0.72506944444444443</v>
       </c>
     </row>
-    <row r="142" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:28">
       <c r="C142" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D142">
         <v>36</v>
@@ -11571,7 +11563,7 @@
         <v>0.72682870370370367</v>
       </c>
     </row>
-    <row r="143" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:28">
       <c r="D143">
         <v>36</v>
       </c>
@@ -11648,7 +11640,7 @@
         <v>0.7268634259259259</v>
       </c>
     </row>
-    <row r="144" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:28">
       <c r="D144">
         <v>36</v>
       </c>
@@ -11725,7 +11717,7 @@
         <v>0.72689814814814813</v>
       </c>
     </row>
-    <row r="145" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:28">
       <c r="D145">
         <v>36</v>
       </c>
@@ -11802,9 +11794,9 @@
         <v>0.72692129629629632</v>
       </c>
     </row>
-    <row r="146" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:28">
       <c r="C146" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D146">
         <v>37</v>
@@ -11882,7 +11874,7 @@
         <v>0.7275462962962963</v>
       </c>
     </row>
-    <row r="147" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:28">
       <c r="D147">
         <v>37</v>
       </c>
@@ -11959,7 +11951,7 @@
         <v>0.72756944444444438</v>
       </c>
     </row>
-    <row r="148" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:28">
       <c r="D148">
         <v>37</v>
       </c>
@@ -12036,7 +12028,7 @@
         <v>0.72760416666666661</v>
       </c>
     </row>
-    <row r="149" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:28">
       <c r="D149">
         <v>37</v>
       </c>
@@ -12113,9 +12105,9 @@
         <v>0.7276273148148148</v>
       </c>
     </row>
-    <row r="150" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:28">
       <c r="C150" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D150">
         <v>38</v>
@@ -12193,7 +12185,7 @@
         <v>0.72805555555555557</v>
       </c>
     </row>
-    <row r="151" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:28">
       <c r="D151">
         <v>38</v>
       </c>
@@ -12270,7 +12262,7 @@
         <v>0.72809027777777768</v>
       </c>
     </row>
-    <row r="152" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:28">
       <c r="D152">
         <v>38</v>
       </c>
@@ -12347,7 +12339,7 @@
         <v>0.72811342592592598</v>
       </c>
     </row>
-    <row r="153" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:28">
       <c r="D153">
         <v>38</v>
       </c>
@@ -12424,9 +12416,9 @@
         <v>0.7281481481481481</v>
       </c>
     </row>
-    <row r="154" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:28">
       <c r="C154" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D154">
         <v>39</v>
@@ -12504,7 +12496,7 @@
         <v>0.72858796296296291</v>
       </c>
     </row>
-    <row r="155" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:28">
       <c r="D155">
         <v>39</v>
       </c>
@@ -12581,7 +12573,7 @@
         <v>0.72863425925925929</v>
       </c>
     </row>
-    <row r="156" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:28">
       <c r="D156">
         <v>39</v>
       </c>
@@ -12658,7 +12650,7 @@
         <v>0.72865740740740748</v>
       </c>
     </row>
-    <row r="157" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:28">
       <c r="D157">
         <v>39</v>
       </c>
@@ -12735,9 +12727,9 @@
         <v>0.72868055555555555</v>
       </c>
     </row>
-    <row r="158" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:28">
       <c r="C158" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D158">
         <v>40</v>
@@ -12815,7 +12807,7 @@
         <v>0.72917824074074078</v>
       </c>
     </row>
-    <row r="159" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:28">
       <c r="D159">
         <v>40</v>
       </c>
@@ -12892,7 +12884,7 @@
         <v>0.72920138888888886</v>
       </c>
     </row>
-    <row r="160" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:28">
       <c r="D160">
         <v>40</v>
       </c>
@@ -12969,7 +12961,7 @@
         <v>0.72922453703703705</v>
       </c>
     </row>
-    <row r="161" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:28">
       <c r="D161">
         <v>40</v>
       </c>
@@ -13046,9 +13038,9 @@
         <v>0.72925925925925927</v>
       </c>
     </row>
-    <row r="162" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:28">
       <c r="C162" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D162">
         <v>41</v>
@@ -13126,7 +13118,7 @@
         <v>0.72966435185185186</v>
       </c>
     </row>
-    <row r="163" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:28">
       <c r="D163">
         <v>41</v>
       </c>
@@ -13203,7 +13195,7 @@
         <v>0.72969907407407408</v>
       </c>
     </row>
-    <row r="164" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:28">
       <c r="D164">
         <v>41</v>
       </c>
@@ -13280,7 +13272,7 @@
         <v>0.72973379629629631</v>
       </c>
     </row>
-    <row r="165" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:28">
       <c r="D165">
         <v>41</v>
       </c>
@@ -13357,15 +13349,15 @@
         <v>0.7297569444444445</v>
       </c>
     </row>
-    <row r="166" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:28">
       <c r="A166">
         <v>6</v>
       </c>
       <c r="B166" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C166" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D166">
         <v>42</v>
@@ -13443,7 +13435,7 @@
         <v>0.73094907407407417</v>
       </c>
     </row>
-    <row r="167" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:28">
       <c r="D167">
         <v>42</v>
       </c>
@@ -13520,7 +13512,7 @@
         <v>0.73098379629629628</v>
       </c>
     </row>
-    <row r="168" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:28">
       <c r="D168">
         <v>42</v>
       </c>
@@ -13597,7 +13589,7 @@
         <v>0.73100694444444436</v>
       </c>
     </row>
-    <row r="169" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:28">
       <c r="D169">
         <v>42</v>
       </c>
@@ -13674,9 +13666,9 @@
         <v>0.7310416666666667</v>
       </c>
     </row>
-    <row r="170" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:28">
       <c r="C170" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D170">
         <v>43</v>
@@ -13754,7 +13746,7 @@
         <v>0.73141203703703705</v>
       </c>
     </row>
-    <row r="171" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:28">
       <c r="D171">
         <v>43</v>
       </c>
@@ -13831,7 +13823,7 @@
         <v>0.73146990740740747</v>
       </c>
     </row>
-    <row r="172" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:28">
       <c r="D172">
         <v>43</v>
       </c>
@@ -13908,7 +13900,7 @@
         <v>0.73149305555555555</v>
       </c>
     </row>
-    <row r="173" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:28">
       <c r="D173">
         <v>43</v>
       </c>
@@ -13985,9 +13977,9 @@
         <v>0.73153935185185182</v>
       </c>
     </row>
-    <row r="174" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:28">
       <c r="C174" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D174">
         <v>44</v>
@@ -14065,7 +14057,7 @@
         <v>0.73458333333333325</v>
       </c>
     </row>
-    <row r="175" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:28">
       <c r="D175">
         <v>44</v>
       </c>
@@ -14142,7 +14134,7 @@
         <v>0.73460648148148155</v>
       </c>
     </row>
-    <row r="176" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:28">
       <c r="D176">
         <v>44</v>
       </c>
@@ -14219,7 +14211,7 @@
         <v>0.73464120370370367</v>
       </c>
     </row>
-    <row r="177" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:28">
       <c r="D177">
         <v>44</v>
       </c>
@@ -14296,9 +14288,9 @@
         <v>0.7346759259259259</v>
       </c>
     </row>
-    <row r="178" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:28">
       <c r="C178" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D178">
         <v>45</v>
@@ -14376,7 +14368,7 @@
         <v>0.7350578703703704</v>
       </c>
     </row>
-    <row r="179" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:28">
       <c r="D179">
         <v>45</v>
       </c>
@@ -14453,7 +14445,7 @@
         <v>0.73508101851851848</v>
       </c>
     </row>
-    <row r="180" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:28">
       <c r="D180">
         <v>45</v>
       </c>
@@ -14530,7 +14522,7 @@
         <v>0.73511574074074071</v>
       </c>
     </row>
-    <row r="181" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:28">
       <c r="D181">
         <v>45</v>
       </c>
@@ -14607,9 +14599,9 @@
         <v>0.7351388888888889</v>
       </c>
     </row>
-    <row r="182" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:28">
       <c r="C182" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D182">
         <v>46</v>
@@ -14687,7 +14679,7 @@
         <v>0.73556712962962967</v>
       </c>
     </row>
-    <row r="183" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:28">
       <c r="D183">
         <v>46</v>
       </c>
@@ -14764,7 +14756,7 @@
         <v>0.73560185185185178</v>
       </c>
     </row>
-    <row r="184" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:28">
       <c r="D184">
         <v>46</v>
       </c>
@@ -14841,7 +14833,7 @@
         <v>0.73562500000000008</v>
       </c>
     </row>
-    <row r="185" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:28">
       <c r="D185">
         <v>46</v>
       </c>
@@ -14918,9 +14910,9 @@
         <v>0.7356597222222222</v>
       </c>
     </row>
-    <row r="186" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:28">
       <c r="C186" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D186">
         <v>47</v>
@@ -14998,7 +14990,7 @@
         <v>0.7361805555555555</v>
       </c>
     </row>
-    <row r="187" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:28">
       <c r="D187">
         <v>47</v>
       </c>
@@ -15075,7 +15067,7 @@
         <v>0.7362037037037038</v>
       </c>
     </row>
-    <row r="188" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:28">
       <c r="D188">
         <v>47</v>
       </c>
@@ -15152,7 +15144,7 @@
         <v>0.73623842592592592</v>
       </c>
     </row>
-    <row r="189" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:28">
       <c r="D189">
         <v>47</v>
       </c>
@@ -15229,9 +15221,9 @@
         <v>0.73627314814814815</v>
       </c>
     </row>
-    <row r="190" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:28">
       <c r="C190" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D190">
         <v>48</v>
@@ -15309,7 +15301,7 @@
         <v>0.73665509259259254</v>
       </c>
     </row>
-    <row r="191" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:28">
       <c r="D191">
         <v>48</v>
       </c>
@@ -15386,7 +15378,7 @@
         <v>0.73668981481481488</v>
       </c>
     </row>
-    <row r="192" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:28">
       <c r="D192">
         <v>48</v>
       </c>
@@ -15463,7 +15455,7 @@
         <v>0.73671296296296296</v>
       </c>
     </row>
-    <row r="193" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:28">
       <c r="D193">
         <v>48</v>
       </c>
@@ -15540,9 +15532,9 @@
         <v>0.73675925925925922</v>
       </c>
     </row>
-    <row r="194" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:28">
       <c r="C194" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D194">
         <v>49</v>
@@ -15620,7 +15612,7 @@
         <v>0.73736111111111102</v>
       </c>
     </row>
-    <row r="195" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:28">
       <c r="D195">
         <v>49</v>
       </c>
@@ -15697,7 +15689,7 @@
         <v>0.7374074074074074</v>
       </c>
     </row>
-    <row r="196" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:28">
       <c r="D196">
         <v>49</v>
       </c>
@@ -15774,7 +15766,7 @@
         <v>0.73743055555555559</v>
       </c>
     </row>
-    <row r="197" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:28">
       <c r="D197">
         <v>49</v>
       </c>
@@ -15851,9 +15843,9 @@
         <v>0.73746527777777782</v>
       </c>
     </row>
-    <row r="198" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:28">
       <c r="C198" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D198">
         <v>50</v>
@@ -15931,7 +15923,7 @@
         <v>0.7379282407407407</v>
       </c>
     </row>
-    <row r="199" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:28">
       <c r="D199">
         <v>50</v>
       </c>
@@ -16008,7 +16000,7 @@
         <v>0.73795138888888889</v>
       </c>
     </row>
-    <row r="200" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:28">
       <c r="D200">
         <v>50</v>
       </c>
@@ -16085,7 +16077,7 @@
         <v>0.73797453703703697</v>
       </c>
     </row>
-    <row r="201" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:28">
       <c r="D201">
         <v>50</v>
       </c>
@@ -16162,9 +16154,9 @@
         <v>0.73800925925925931</v>
       </c>
     </row>
-    <row r="202" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:28">
       <c r="C202" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D202">
         <v>51</v>
@@ -16242,7 +16234,7 @@
         <v>0.73842592592592593</v>
       </c>
     </row>
-    <row r="203" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:28">
       <c r="D203">
         <v>51</v>
       </c>
@@ -16319,7 +16311,7 @@
         <v>0.73846064814814805</v>
       </c>
     </row>
-    <row r="204" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:28">
       <c r="D204">
         <v>51</v>
       </c>
@@ -16396,7 +16388,7 @@
         <v>0.73849537037037039</v>
       </c>
     </row>
-    <row r="205" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:28">
       <c r="D205">
         <v>51</v>
       </c>
@@ -16473,9 +16465,9 @@
         <v>0.73851851851851846</v>
       </c>
     </row>
-    <row r="206" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="206" spans="3:28">
       <c r="C206" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D206">
         <v>52</v>
@@ -16553,7 +16545,7 @@
         <v>0.73916666666666664</v>
       </c>
     </row>
-    <row r="207" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="207" spans="3:28">
       <c r="D207">
         <v>52</v>
       </c>
@@ -16630,7 +16622,7 @@
         <v>0.73920138888888898</v>
       </c>
     </row>
-    <row r="208" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="208" spans="3:28">
       <c r="D208">
         <v>52</v>
       </c>
@@ -16707,7 +16699,7 @@
         <v>0.73922453703703705</v>
       </c>
     </row>
-    <row r="209" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:28">
       <c r="D209">
         <v>52</v>
       </c>
@@ -16784,9 +16776,9 @@
         <v>0.73924768518518524</v>
       </c>
     </row>
-    <row r="210" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:28">
       <c r="C210" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D210">
         <v>53</v>
@@ -16864,7 +16856,7 @@
         <v>0.73961805555555549</v>
       </c>
     </row>
-    <row r="211" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:28">
       <c r="D211">
         <v>53</v>
       </c>
@@ -16941,7 +16933,7 @@
         <v>0.73964120370370379</v>
       </c>
     </row>
-    <row r="212" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:28">
       <c r="D212">
         <v>53</v>
       </c>
@@ -17018,7 +17010,7 @@
         <v>0.73968750000000005</v>
       </c>
     </row>
-    <row r="213" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:28">
       <c r="D213">
         <v>53</v>
       </c>
@@ -17095,9 +17087,9 @@
         <v>0.73971064814814813</v>
       </c>
     </row>
-    <row r="214" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:28">
       <c r="C214" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D214">
         <v>54</v>
@@ -17175,7 +17167,7 @@
         <v>0.74018518518518517</v>
       </c>
     </row>
-    <row r="215" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:28">
       <c r="D215">
         <v>54</v>
       </c>
@@ -17252,7 +17244,7 @@
         <v>0.74021990740740751</v>
       </c>
     </row>
-    <row r="216" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:28">
       <c r="D216">
         <v>54</v>
       </c>
@@ -17329,7 +17321,7 @@
         <v>0.74024305555555558</v>
       </c>
     </row>
-    <row r="217" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:28">
       <c r="D217">
         <v>54</v>
       </c>
@@ -17406,9 +17398,9 @@
         <v>0.74031249999999993</v>
       </c>
     </row>
-    <row r="218" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:28">
       <c r="C218" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D218">
         <v>55</v>
@@ -17486,7 +17478,7 @@
         <v>0.74072916666666666</v>
       </c>
     </row>
-    <row r="219" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:28">
       <c r="D219">
         <v>55</v>
       </c>
@@ -17563,7 +17555,7 @@
         <v>0.74075231481481474</v>
       </c>
     </row>
-    <row r="220" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:28">
       <c r="D220">
         <v>55</v>
       </c>
@@ -17640,7 +17632,7 @@
         <v>0.74078703703703708</v>
       </c>
     </row>
-    <row r="221" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:28">
       <c r="D221">
         <v>55</v>
       </c>
@@ -17717,9 +17709,9 @@
         <v>0.74081018518518515</v>
       </c>
     </row>
-    <row r="222" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:28">
       <c r="C222" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D222">
         <v>56</v>
@@ -17797,7 +17789,7 @@
         <v>0.74124999999999996</v>
       </c>
     </row>
-    <row r="223" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:28">
       <c r="D223">
         <v>56</v>
       </c>
@@ -17874,7 +17866,7 @@
         <v>0.74128472222222219</v>
       </c>
     </row>
-    <row r="224" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:28">
       <c r="D224">
         <v>56</v>
       </c>
@@ -17951,7 +17943,7 @@
         <v>0.74130787037037038</v>
       </c>
     </row>
-    <row r="225" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:28">
       <c r="D225">
         <v>56</v>
       </c>
@@ -18028,9 +18020,9 @@
         <v>0.7413657407407408</v>
       </c>
     </row>
-    <row r="226" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:28">
       <c r="C226" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D226">
         <v>57</v>
@@ -18108,7 +18100,7 @@
         <v>0.74202546296296301</v>
       </c>
     </row>
-    <row r="227" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:28">
       <c r="D227">
         <v>57</v>
       </c>
@@ -18185,7 +18177,7 @@
         <v>0.74206018518518524</v>
       </c>
     </row>
-    <row r="228" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:28">
       <c r="D228">
         <v>57</v>
       </c>
@@ -18262,7 +18254,7 @@
         <v>0.74209490740740736</v>
       </c>
     </row>
-    <row r="229" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:28">
       <c r="D229">
         <v>57</v>
       </c>
@@ -18339,9 +18331,9 @@
         <v>0.74212962962962958</v>
       </c>
     </row>
-    <row r="230" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:28">
       <c r="C230" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D230">
         <v>58</v>
@@ -18419,7 +18411,7 @@
         <v>0.74662037037037043</v>
       </c>
     </row>
-    <row r="231" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:28">
       <c r="D231">
         <v>58</v>
       </c>
@@ -18496,7 +18488,7 @@
         <v>0.74664351851851851</v>
       </c>
     </row>
-    <row r="232" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:28">
       <c r="D232">
         <v>58</v>
       </c>
@@ -18573,7 +18565,7 @@
         <v>0.7466666666666667</v>
       </c>
     </row>
-    <row r="233" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:28">
       <c r="D233">
         <v>58</v>
       </c>
@@ -18650,9 +18642,9 @@
         <v>0.74670138888888893</v>
       </c>
     </row>
-    <row r="234" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:28">
       <c r="C234" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D234">
         <v>59</v>
@@ -18730,7 +18722,7 @@
         <v>0.74712962962962959</v>
       </c>
     </row>
-    <row r="235" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:28">
       <c r="D235">
         <v>59</v>
       </c>
@@ -18807,7 +18799,7 @@
         <v>0.74716435185185182</v>
       </c>
     </row>
-    <row r="236" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:28">
       <c r="D236">
         <v>59</v>
       </c>
@@ -18884,7 +18876,7 @@
         <v>0.74719907407407404</v>
       </c>
     </row>
-    <row r="237" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:28">
       <c r="D237">
         <v>59</v>
       </c>
@@ -18961,9 +18953,9 @@
         <v>0.74722222222222223</v>
       </c>
     </row>
-    <row r="238" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="238" spans="3:28">
       <c r="C238" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D238">
         <v>60</v>
@@ -19041,7 +19033,7 @@
         <v>0.74782407407407403</v>
       </c>
     </row>
-    <row r="239" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="239" spans="3:28">
       <c r="D239">
         <v>60</v>
       </c>
@@ -19118,7 +19110,7 @@
         <v>0.74784722222222222</v>
       </c>
     </row>
-    <row r="240" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="240" spans="3:28">
       <c r="D240">
         <v>60</v>
       </c>
@@ -19195,7 +19187,7 @@
         <v>0.7478703703703703</v>
       </c>
     </row>
-    <row r="241" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:28">
       <c r="D241">
         <v>60</v>
       </c>
@@ -19272,9 +19264,9 @@
         <v>0.74790509259259252</v>
       </c>
     </row>
-    <row r="242" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:28">
       <c r="C242" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D242">
         <v>61</v>
@@ -19352,7 +19344,7 @@
         <v>0.74826388888888884</v>
       </c>
     </row>
-    <row r="243" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:28">
       <c r="D243">
         <v>61</v>
       </c>
@@ -19429,7 +19421,7 @@
         <v>0.74829861111111118</v>
       </c>
     </row>
-    <row r="244" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:28">
       <c r="D244">
         <v>61</v>
       </c>
@@ -19506,7 +19498,7 @@
         <v>0.74833333333333341</v>
       </c>
     </row>
-    <row r="245" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:28">
       <c r="D245">
         <v>61</v>
       </c>
@@ -19583,15 +19575,15 @@
         <v>0.74835648148148148</v>
       </c>
     </row>
-    <row r="246" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:28">
       <c r="A246">
         <v>7</v>
       </c>
       <c r="B246" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C246" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D246">
         <v>62</v>
@@ -19669,7 +19661,7 @@
         <v>0.74903935185185189</v>
       </c>
     </row>
-    <row r="247" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:28">
       <c r="D247">
         <v>62</v>
       </c>
@@ -19746,7 +19738,7 @@
         <v>0.74906249999999996</v>
       </c>
     </row>
-    <row r="248" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:28">
       <c r="D248">
         <v>62</v>
       </c>
@@ -19823,7 +19815,7 @@
         <v>0.74910879629629623</v>
       </c>
     </row>
-    <row r="249" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:28">
       <c r="D249">
         <v>62</v>
       </c>
@@ -19900,9 +19892,9 @@
         <v>0.74913194444444453</v>
       </c>
     </row>
-    <row r="250" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:28">
       <c r="C250" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D250">
         <v>63</v>
@@ -19980,7 +19972,7 @@
         <v>0.74956018518518519</v>
       </c>
     </row>
-    <row r="251" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:28">
       <c r="D251">
         <v>63</v>
       </c>
@@ -20057,7 +20049,7 @@
         <v>0.74959490740740742</v>
       </c>
     </row>
-    <row r="252" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:28">
       <c r="D252">
         <v>63</v>
       </c>
@@ -20134,7 +20126,7 @@
         <v>0.74962962962962953</v>
       </c>
     </row>
-    <row r="253" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:28">
       <c r="D253">
         <v>63</v>
       </c>
@@ -20211,9 +20203,9 @@
         <v>0.74967592592592591</v>
       </c>
     </row>
-    <row r="254" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:28">
       <c r="C254" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D254">
         <v>64</v>
@@ -20291,7 +20283,7 @@
         <v>0.75002314814814808</v>
       </c>
     </row>
-    <row r="255" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:28">
       <c r="D255">
         <v>64</v>
       </c>
@@ -20368,7 +20360,7 @@
         <v>0.75005787037037042</v>
       </c>
     </row>
-    <row r="256" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:28">
       <c r="D256">
         <v>64</v>
       </c>
@@ -20445,7 +20437,7 @@
         <v>0.75008101851851849</v>
       </c>
     </row>
-    <row r="257" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="257" spans="3:28">
       <c r="D257">
         <v>64</v>
       </c>
@@ -20522,9 +20514,9 @@
         <v>0.75011574074074072</v>
       </c>
     </row>
-    <row r="258" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="258" spans="3:28">
       <c r="C258" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D258">
         <v>65</v>
@@ -20602,7 +20594,7 @@
         <v>0.75054398148148149</v>
       </c>
     </row>
-    <row r="259" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="259" spans="3:28">
       <c r="D259">
         <v>65</v>
       </c>
@@ -20679,7 +20671,7 @@
         <v>0.75057870370370372</v>
       </c>
     </row>
-    <row r="260" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="260" spans="3:28">
       <c r="D260">
         <v>65</v>
       </c>
@@ -20756,7 +20748,7 @@
         <v>0.7506018518518518</v>
       </c>
     </row>
-    <row r="261" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="261" spans="3:28">
       <c r="D261">
         <v>65</v>
       </c>
@@ -20833,9 +20825,9 @@
         <v>0.75063657407407414</v>
       </c>
     </row>
-    <row r="262" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="262" spans="3:28">
       <c r="C262" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D262">
         <v>66</v>
@@ -20913,7 +20905,7 @@
         <v>0.7510648148148148</v>
       </c>
     </row>
-    <row r="263" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="263" spans="3:28">
       <c r="D263">
         <v>66</v>
       </c>
@@ -20990,7 +20982,7 @@
         <v>0.75108796296296287</v>
       </c>
     </row>
-    <row r="264" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="264" spans="3:28">
       <c r="D264">
         <v>66</v>
       </c>
@@ -21067,7 +21059,7 @@
         <v>0.75111111111111117</v>
       </c>
     </row>
-    <row r="265" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="265" spans="3:28">
       <c r="D265">
         <v>66</v>
       </c>
@@ -21144,9 +21136,9 @@
         <v>0.75114583333333329</v>
       </c>
     </row>
-    <row r="266" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="266" spans="3:28">
       <c r="C266" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D266">
         <v>67</v>
@@ -21224,7 +21216,7 @@
         <v>0.75208333333333333</v>
       </c>
     </row>
-    <row r="267" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="267" spans="3:28">
       <c r="D267">
         <v>67</v>
       </c>
@@ -21301,7 +21293,7 @@
         <v>0.7521296296296297</v>
       </c>
     </row>
-    <row r="268" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="268" spans="3:28">
       <c r="D268">
         <v>67</v>
       </c>
@@ -21378,7 +21370,7 @@
         <v>0.75215277777777778</v>
       </c>
     </row>
-    <row r="269" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="269" spans="3:28">
       <c r="D269">
         <v>67</v>
       </c>
@@ -21455,9 +21447,9 @@
         <v>0.75217592592592597</v>
       </c>
     </row>
-    <row r="270" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="270" spans="3:28">
       <c r="C270" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D270">
         <v>68</v>
@@ -21535,7 +21527,7 @@
         <v>0.75261574074074078</v>
       </c>
     </row>
-    <row r="271" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="271" spans="3:28">
       <c r="D271">
         <v>68</v>
       </c>
@@ -21612,7 +21604,7 @@
         <v>0.75263888888888886</v>
       </c>
     </row>
-    <row r="272" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="272" spans="3:28">
       <c r="D272">
         <v>68</v>
       </c>
@@ -21689,7 +21681,7 @@
         <v>0.75267361111111108</v>
       </c>
     </row>
-    <row r="273" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:28">
       <c r="D273">
         <v>68</v>
       </c>
@@ -21766,9 +21758,9 @@
         <v>0.75270833333333342</v>
       </c>
     </row>
-    <row r="274" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="274" spans="3:28">
       <c r="C274" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D274">
         <v>69</v>
@@ -21846,7 +21838,7 @@
         <v>0.75306712962962974</v>
       </c>
     </row>
-    <row r="275" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:28">
       <c r="D275">
         <v>69</v>
       </c>
@@ -21923,7 +21915,7 @@
         <v>0.75309027777777782</v>
       </c>
     </row>
-    <row r="276" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:28">
       <c r="D276">
         <v>69</v>
       </c>
@@ -22000,7 +21992,7 @@
         <v>0.75313657407407408</v>
       </c>
     </row>
-    <row r="277" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:28">
       <c r="D277">
         <v>69</v>
       </c>
@@ -22077,9 +22069,9 @@
         <v>0.75317129629629631</v>
       </c>
     </row>
-    <row r="278" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="278" spans="3:28">
       <c r="C278" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D278">
         <v>70</v>
@@ -22157,7 +22149,7 @@
         <v>0.75357638888888889</v>
       </c>
     </row>
-    <row r="279" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="279" spans="3:28">
       <c r="D279">
         <v>70</v>
       </c>
@@ -22234,7 +22226,7 @@
         <v>0.75361111111111112</v>
       </c>
     </row>
-    <row r="280" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:28">
       <c r="D280">
         <v>70</v>
       </c>
@@ -22311,7 +22303,7 @@
         <v>0.75363425925925931</v>
       </c>
     </row>
-    <row r="281" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:28">
       <c r="D281">
         <v>70</v>
       </c>
@@ -22388,9 +22380,9 @@
         <v>0.75366898148148154</v>
       </c>
     </row>
-    <row r="282" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:28">
       <c r="C282" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D282">
         <v>71</v>
@@ -22468,7 +22460,7 @@
         <v>0.75406249999999997</v>
       </c>
     </row>
-    <row r="283" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:28">
       <c r="D283">
         <v>71</v>
       </c>
@@ -22545,7 +22537,7 @@
         <v>0.75407407407407412</v>
       </c>
     </row>
-    <row r="284" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:28">
       <c r="D284">
         <v>71</v>
       </c>
@@ -22622,7 +22614,7 @@
         <v>0.7540972222222222</v>
       </c>
     </row>
-    <row r="285" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:28">
       <c r="D285">
         <v>71</v>
       </c>
@@ -22699,9 +22691,9 @@
         <v>0.75413194444444442</v>
       </c>
     </row>
-    <row r="286" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="286" spans="3:28">
       <c r="C286" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D286">
         <v>72</v>
@@ -22779,7 +22771,7 @@
         <v>0.75465277777777784</v>
       </c>
     </row>
-    <row r="287" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="287" spans="3:28">
       <c r="D287">
         <v>72</v>
       </c>
@@ -22856,7 +22848,7 @@
         <v>0.75468750000000007</v>
       </c>
     </row>
-    <row r="288" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="288" spans="3:28">
       <c r="D288">
         <v>72</v>
       </c>
@@ -22933,7 +22925,7 @@
         <v>0.75472222222222218</v>
       </c>
     </row>
-    <row r="289" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:28">
       <c r="D289">
         <v>72</v>
       </c>
@@ -23010,9 +23002,9 @@
         <v>0.75475694444444441</v>
       </c>
     </row>
-    <row r="290" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:28">
       <c r="C290" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D290">
         <v>73</v>
@@ -23090,7 +23082,7 @@
         <v>0.75553240740740746</v>
       </c>
     </row>
-    <row r="291" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:28">
       <c r="D291">
         <v>73</v>
       </c>
@@ -23167,7 +23159,7 @@
         <v>0.75555555555555554</v>
       </c>
     </row>
-    <row r="292" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:28">
       <c r="D292">
         <v>73</v>
       </c>
@@ -23244,7 +23236,7 @@
         <v>0.7556018518518518</v>
       </c>
     </row>
-    <row r="293" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:28">
       <c r="D293">
         <v>73</v>
       </c>
@@ -23321,9 +23313,9 @@
         <v>0.75563657407407403</v>
       </c>
     </row>
-    <row r="294" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:28">
       <c r="C294" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D294">
         <v>74</v>
@@ -23401,7 +23393,7 @@
         <v>0.75618055555555552</v>
       </c>
     </row>
-    <row r="295" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="295" spans="3:28">
       <c r="D295">
         <v>74</v>
       </c>
@@ -23478,7 +23470,7 @@
         <v>0.75621527777777775</v>
       </c>
     </row>
-    <row r="296" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="296" spans="3:28">
       <c r="D296">
         <v>74</v>
       </c>
@@ -23555,7 +23547,7 @@
         <v>0.75624999999999998</v>
       </c>
     </row>
-    <row r="297" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="297" spans="3:28">
       <c r="D297">
         <v>74</v>
       </c>
@@ -23632,9 +23624,9 @@
         <v>0.75629629629629624</v>
       </c>
     </row>
-    <row r="298" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="298" spans="3:28">
       <c r="C298" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D298">
         <v>75</v>
@@ -23712,7 +23704,7 @@
         <v>0.7567476851851852</v>
       </c>
     </row>
-    <row r="299" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:28">
       <c r="D299">
         <v>75</v>
       </c>
@@ -23789,7 +23781,7 @@
         <v>0.75677083333333339</v>
       </c>
     </row>
-    <row r="300" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:28">
       <c r="D300">
         <v>75</v>
       </c>
@@ -23866,7 +23858,7 @@
         <v>0.75679398148148147</v>
       </c>
     </row>
-    <row r="301" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:28">
       <c r="D301">
         <v>75</v>
       </c>
@@ -23943,9 +23935,9 @@
         <v>0.75681712962962966</v>
       </c>
     </row>
-    <row r="302" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="302" spans="3:28">
       <c r="C302" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D302">
         <v>76</v>
@@ -24023,7 +24015,7 @@
         <v>0.75717592592592586</v>
       </c>
     </row>
-    <row r="303" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="303" spans="3:28">
       <c r="D303">
         <v>76</v>
       </c>
@@ -24100,7 +24092,7 @@
         <v>0.75719907407407405</v>
       </c>
     </row>
-    <row r="304" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="304" spans="3:28">
       <c r="D304">
         <v>76</v>
       </c>
@@ -24177,7 +24169,7 @@
         <v>0.75723379629629628</v>
       </c>
     </row>
-    <row r="305" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="305" spans="3:28">
       <c r="D305">
         <v>76</v>
       </c>
@@ -24254,9 +24246,9 @@
         <v>0.75725694444444447</v>
       </c>
     </row>
-    <row r="306" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="306" spans="3:28">
       <c r="C306" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D306">
         <v>77</v>
@@ -24334,7 +24326,7 @@
         <v>0.75782407407407415</v>
       </c>
     </row>
-    <row r="307" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="307" spans="3:28">
       <c r="D307">
         <v>77</v>
       </c>
@@ -24411,7 +24403,7 @@
         <v>0.75785879629629627</v>
       </c>
     </row>
-    <row r="308" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:28">
       <c r="D308">
         <v>77</v>
       </c>
@@ -24488,7 +24480,7 @@
         <v>0.75788194444444434</v>
       </c>
     </row>
-    <row r="309" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:28">
       <c r="D309">
         <v>77</v>
       </c>
@@ -24565,9 +24557,9 @@
         <v>0.75791666666666668</v>
       </c>
     </row>
-    <row r="310" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:28">
       <c r="C310" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D310">
         <v>78</v>
@@ -24645,7 +24637,7 @@
         <v>0.75832175925925915</v>
       </c>
     </row>
-    <row r="311" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:28">
       <c r="D311">
         <v>78</v>
       </c>
@@ -24722,7 +24714,7 @@
         <v>0.75834490740740745</v>
       </c>
     </row>
-    <row r="312" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="312" spans="3:28">
       <c r="D312">
         <v>78</v>
       </c>
@@ -24799,7 +24791,7 @@
         <v>0.75837962962962957</v>
       </c>
     </row>
-    <row r="313" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="313" spans="3:28">
       <c r="D313">
         <v>78</v>
       </c>
@@ -24876,9 +24868,9 @@
         <v>0.75840277777777787</v>
       </c>
     </row>
-    <row r="314" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="314" spans="3:28">
       <c r="C314" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D314">
         <v>79</v>
@@ -24956,7 +24948,7 @@
         <v>0.75888888888888895</v>
       </c>
     </row>
-    <row r="315" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="315" spans="3:28">
       <c r="D315">
         <v>79</v>
       </c>
@@ -25033,7 +25025,7 @@
         <v>0.75891203703703702</v>
       </c>
     </row>
-    <row r="316" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="316" spans="3:28">
       <c r="D316">
         <v>79</v>
       </c>
@@ -25110,7 +25102,7 @@
         <v>0.75895833333333329</v>
       </c>
     </row>
-    <row r="317" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="317" spans="3:28">
       <c r="D317">
         <v>79</v>
       </c>
@@ -25187,9 +25179,9 @@
         <v>0.75898148148148159</v>
       </c>
     </row>
-    <row r="318" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="318" spans="3:28">
       <c r="C318" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D318">
         <v>80</v>
@@ -25267,7 +25259,7 @@
         <v>0.75937500000000002</v>
       </c>
     </row>
-    <row r="319" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="319" spans="3:28">
       <c r="D319">
         <v>80</v>
       </c>
@@ -25344,7 +25336,7 @@
         <v>0.7593981481481481</v>
       </c>
     </row>
-    <row r="320" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="320" spans="3:28">
       <c r="D320">
         <v>80</v>
       </c>
@@ -25421,7 +25413,7 @@
         <v>0.75943287037037033</v>
       </c>
     </row>
-    <row r="321" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:28">
       <c r="D321">
         <v>80</v>
       </c>
@@ -25498,9 +25490,9 @@
         <v>0.75945601851851852</v>
       </c>
     </row>
-    <row r="322" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:28">
       <c r="C322" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D322">
         <v>81</v>
@@ -25578,7 +25570,7 @@
         <v>0.75987268518518514</v>
       </c>
     </row>
-    <row r="323" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:28">
       <c r="D323">
         <v>81</v>
       </c>
@@ -25655,7 +25647,7 @@
         <v>0.75989583333333333</v>
       </c>
     </row>
-    <row r="324" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:28">
       <c r="D324">
         <v>81</v>
       </c>
@@ -25732,7 +25724,7 @@
         <v>0.7599189814814814</v>
       </c>
     </row>
-    <row r="325" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:28">
       <c r="D325">
         <v>81</v>
       </c>
@@ -25809,15 +25801,15 @@
         <v>0.75995370370370363</v>
       </c>
     </row>
-    <row r="326" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:28">
       <c r="A326">
         <v>8</v>
       </c>
       <c r="B326" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C326" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D326">
         <v>82</v>
@@ -25895,7 +25887,7 @@
         <v>0.76079861111111102</v>
       </c>
     </row>
-    <row r="327" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:28">
       <c r="D327">
         <v>82</v>
       </c>
@@ -25972,7 +25964,7 @@
         <v>0.76082175925925932</v>
       </c>
     </row>
-    <row r="328" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:28">
       <c r="D328">
         <v>82</v>
       </c>
@@ -26049,7 +26041,7 @@
         <v>0.76085648148148144</v>
       </c>
     </row>
-    <row r="329" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:28">
       <c r="D329">
         <v>82</v>
       </c>
@@ -26126,9 +26118,9 @@
         <v>0.76087962962962974</v>
       </c>
     </row>
-    <row r="330" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:28">
       <c r="C330" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D330">
         <v>83</v>
@@ -26206,7 +26198,7 @@
         <v>0.76128472222222221</v>
       </c>
     </row>
-    <row r="331" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:28">
       <c r="D331">
         <v>83</v>
       </c>
@@ -26283,7 +26275,7 @@
         <v>0.76131944444444455</v>
       </c>
     </row>
-    <row r="332" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:28">
       <c r="D332">
         <v>83</v>
       </c>
@@ -26360,7 +26352,7 @@
         <v>0.76134259259259263</v>
       </c>
     </row>
-    <row r="333" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:28">
       <c r="D333">
         <v>83</v>
       </c>
@@ -26437,9 +26429,9 @@
         <v>0.7613657407407407</v>
       </c>
     </row>
-    <row r="334" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:28">
       <c r="C334" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D334">
         <v>84</v>
@@ -26517,7 +26509,7 @@
         <v>0.76429398148148142</v>
       </c>
     </row>
-    <row r="335" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:28">
       <c r="D335">
         <v>84</v>
       </c>
@@ -26594,7 +26586,7 @@
         <v>0.7643402777777778</v>
       </c>
     </row>
-    <row r="336" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:28">
       <c r="D336">
         <v>84</v>
       </c>
@@ -26671,7 +26663,7 @@
         <v>0.76437499999999992</v>
       </c>
     </row>
-    <row r="337" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="337" spans="3:28">
       <c r="D337">
         <v>84</v>
       </c>
@@ -26748,9 +26740,9 @@
         <v>0.76440972222222225</v>
       </c>
     </row>
-    <row r="338" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="338" spans="3:28">
       <c r="C338" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D338">
         <v>85</v>
@@ -26828,7 +26820,7 @@
         <v>0.76508101851851851</v>
       </c>
     </row>
-    <row r="339" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="339" spans="3:28">
       <c r="D339">
         <v>85</v>
       </c>
@@ -26905,7 +26897,7 @@
         <v>0.76511574074074085</v>
       </c>
     </row>
-    <row r="340" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="340" spans="3:28">
       <c r="D340">
         <v>85</v>
       </c>
@@ -26982,7 +26974,7 @@
         <v>0.76515046296296296</v>
       </c>
     </row>
-    <row r="341" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="341" spans="3:28">
       <c r="D341">
         <v>85</v>
       </c>
@@ -27059,9 +27051,9 @@
         <v>0.76517361111111104</v>
       </c>
     </row>
-    <row r="342" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="342" spans="3:28">
       <c r="C342" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D342">
         <v>86</v>
@@ -27139,7 +27131,7 @@
         <v>0.76559027777777777</v>
       </c>
     </row>
-    <row r="343" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="343" spans="3:28">
       <c r="D343">
         <v>86</v>
       </c>
@@ -27216,7 +27208,7 @@
         <v>0.765625</v>
       </c>
     </row>
-    <row r="344" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="344" spans="3:28">
       <c r="D344">
         <v>86</v>
       </c>
@@ -27293,7 +27285,7 @@
         <v>0.76565972222222223</v>
       </c>
     </row>
-    <row r="345" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="345" spans="3:28">
       <c r="D345">
         <v>86</v>
       </c>
@@ -27370,9 +27362,9 @@
         <v>0.76569444444444434</v>
       </c>
     </row>
-    <row r="346" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="346" spans="3:28">
       <c r="C346" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D346">
         <v>87</v>
@@ -27450,7 +27442,7 @@
         <v>0.76628472222222221</v>
       </c>
     </row>
-    <row r="347" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="347" spans="3:28">
       <c r="D347">
         <v>87</v>
       </c>
@@ -27527,7 +27519,7 @@
         <v>0.76631944444444444</v>
       </c>
     </row>
-    <row r="348" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="348" spans="3:28">
       <c r="D348">
         <v>87</v>
       </c>
@@ -27604,7 +27596,7 @@
         <v>0.76634259259259263</v>
       </c>
     </row>
-    <row r="349" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="349" spans="3:28">
       <c r="D349">
         <v>87</v>
       </c>
@@ -27681,9 +27673,9 @@
         <v>0.76637731481481486</v>
       </c>
     </row>
-    <row r="350" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="350" spans="3:28">
       <c r="C350" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D350">
         <v>88</v>
@@ -27761,7 +27753,7 @@
         <v>0.76673611111111117</v>
       </c>
     </row>
-    <row r="351" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="351" spans="3:28">
       <c r="D351">
         <v>88</v>
       </c>
@@ -27838,7 +27830,7 @@
         <v>0.76677083333333329</v>
       </c>
     </row>
-    <row r="352" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="352" spans="3:28">
       <c r="D352">
         <v>88</v>
       </c>
@@ -27915,7 +27907,7 @@
         <v>0.76680555555555552</v>
       </c>
     </row>
-    <row r="353" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:28">
       <c r="D353">
         <v>88</v>
       </c>
@@ -27992,9 +27984,9 @@
         <v>0.76682870370370371</v>
       </c>
     </row>
-    <row r="354" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:28">
       <c r="C354" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D354">
         <v>89</v>
@@ -28072,7 +28064,7 @@
         <v>0.76725694444444448</v>
       </c>
     </row>
-    <row r="355" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:28">
       <c r="D355">
         <v>89</v>
       </c>
@@ -28149,7 +28141,7 @@
         <v>0.76731481481481489</v>
       </c>
     </row>
-    <row r="356" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="356" spans="3:28">
       <c r="D356">
         <v>89</v>
       </c>
@@ -28226,7 +28218,7 @@
         <v>0.76734953703703701</v>
       </c>
     </row>
-    <row r="357" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:28">
       <c r="D357">
         <v>89</v>
       </c>
@@ -28303,9 +28295,9 @@
         <v>0.76737268518518509</v>
       </c>
     </row>
-    <row r="358" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="358" spans="3:28">
       <c r="C358" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D358">
         <v>90</v>
@@ -28383,7 +28375,7 @@
         <v>0.76777777777777778</v>
       </c>
     </row>
-    <row r="359" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="359" spans="3:28">
       <c r="D359">
         <v>90</v>
       </c>
@@ -28460,7 +28452,7 @@
         <v>0.76780092592592597</v>
       </c>
     </row>
-    <row r="360" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:28">
       <c r="D360">
         <v>90</v>
       </c>
@@ -28537,7 +28529,7 @@
         <v>0.76782407407407405</v>
       </c>
     </row>
-    <row r="361" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="361" spans="3:28">
       <c r="D361">
         <v>90</v>
       </c>
@@ -28614,9 +28606,9 @@
         <v>0.76785879629629628</v>
       </c>
     </row>
-    <row r="362" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:28">
       <c r="C362" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D362">
         <v>91</v>
@@ -28694,7 +28686,7 @@
         <v>0.76827546296296301</v>
       </c>
     </row>
-    <row r="363" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="363" spans="3:28">
       <c r="D363">
         <v>91</v>
       </c>
@@ -28771,7 +28763,7 @@
         <v>0.76831018518518512</v>
       </c>
     </row>
-    <row r="364" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="364" spans="3:28">
       <c r="D364">
         <v>91</v>
       </c>
@@ -28848,7 +28840,7 @@
         <v>0.76836805555555554</v>
       </c>
     </row>
-    <row r="365" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:28">
       <c r="D365">
         <v>91</v>
       </c>
@@ -28925,9 +28917,9 @@
         <v>0.76839120370370362</v>
       </c>
     </row>
-    <row r="366" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="366" spans="3:28">
       <c r="C366" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D366">
         <v>92</v>
@@ -29005,7 +28997,7 @@
         <v>0.76913194444444455</v>
       </c>
     </row>
-    <row r="367" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="367" spans="3:28">
       <c r="D367">
         <v>92</v>
       </c>
@@ -29082,7 +29074,7 @@
         <v>0.7691782407407407</v>
       </c>
     </row>
-    <row r="368" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="368" spans="3:28">
       <c r="D368">
         <v>92</v>
       </c>
@@ -29159,7 +29151,7 @@
         <v>0.76927083333333324</v>
       </c>
     </row>
-    <row r="369" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:28">
       <c r="D369">
         <v>92</v>
       </c>
@@ -29236,9 +29228,9 @@
         <v>0.76930555555555558</v>
       </c>
     </row>
-    <row r="370" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:28">
       <c r="C370" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D370">
         <v>93</v>
@@ -29316,7 +29308,7 @@
         <v>0.76974537037037039</v>
       </c>
     </row>
-    <row r="371" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:28">
       <c r="D371">
         <v>93</v>
       </c>
@@ -29393,7 +29385,7 @@
         <v>0.76978009259259261</v>
       </c>
     </row>
-    <row r="372" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="372" spans="3:28">
       <c r="D372">
         <v>93</v>
       </c>
@@ -29470,7 +29462,7 @@
         <v>0.76981481481481484</v>
       </c>
     </row>
-    <row r="373" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="373" spans="3:28">
       <c r="D373">
         <v>93</v>
       </c>
@@ -29547,9 +29539,9 @@
         <v>0.76984953703703696</v>
       </c>
     </row>
-    <row r="374" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="374" spans="3:28">
       <c r="C374" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D374">
         <v>94</v>
@@ -29627,7 +29619,7 @@
         <v>0.77026620370370369</v>
       </c>
     </row>
-    <row r="375" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="375" spans="3:28">
       <c r="D375">
         <v>94</v>
       </c>
@@ -29704,7 +29696,7 @@
         <v>0.77028935185185177</v>
       </c>
     </row>
-    <row r="376" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="376" spans="3:28">
       <c r="D376">
         <v>94</v>
       </c>
@@ -29781,7 +29773,7 @@
         <v>0.77032407407407411</v>
       </c>
     </row>
-    <row r="377" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="377" spans="3:28">
       <c r="D377">
         <v>94</v>
       </c>
@@ -29858,9 +29850,9 @@
         <v>0.77035879629629633</v>
       </c>
     </row>
-    <row r="378" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="378" spans="3:28">
       <c r="C378" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D378">
         <v>95</v>
@@ -29938,7 +29930,7 @@
         <v>0.77071759259259265</v>
       </c>
     </row>
-    <row r="379" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="379" spans="3:28">
       <c r="D379">
         <v>95</v>
       </c>
@@ -30015,7 +30007,7 @@
         <v>0.77075231481481488</v>
       </c>
     </row>
-    <row r="380" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="380" spans="3:28">
       <c r="D380">
         <v>95</v>
       </c>
@@ -30092,7 +30084,7 @@
         <v>0.77078703703703699</v>
       </c>
     </row>
-    <row r="381" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="381" spans="3:28">
       <c r="D381">
         <v>95</v>
       </c>
@@ -30169,9 +30161,9 @@
         <v>0.77082175925925922</v>
       </c>
     </row>
-    <row r="382" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="382" spans="3:28">
       <c r="C382" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D382">
         <v>96</v>
@@ -30249,7 +30241,7 @@
         <v>0.77123842592592595</v>
       </c>
     </row>
-    <row r="383" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="383" spans="3:28">
       <c r="D383">
         <v>96</v>
       </c>
@@ -30326,7 +30318,7 @@
         <v>0.77126157407407403</v>
       </c>
     </row>
-    <row r="384" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="384" spans="3:28">
       <c r="D384">
         <v>96</v>
       </c>
@@ -30403,7 +30395,7 @@
         <v>0.77128472222222222</v>
       </c>
     </row>
-    <row r="385" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="385" spans="3:28">
       <c r="D385">
         <v>96</v>
       </c>
@@ -30480,9 +30472,9 @@
         <v>0.77131944444444445</v>
       </c>
     </row>
-    <row r="386" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="386" spans="3:28">
       <c r="C386" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D386">
         <v>97</v>
@@ -30560,7 +30552,7 @@
         <v>0.77186342592592594</v>
       </c>
     </row>
-    <row r="387" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="387" spans="3:28">
       <c r="D387">
         <v>97</v>
       </c>
@@ -30637,7 +30629,7 @@
         <v>0.77189814814814817</v>
       </c>
     </row>
-    <row r="388" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="388" spans="3:28">
       <c r="D388">
         <v>97</v>
       </c>
@@ -30714,7 +30706,7 @@
         <v>0.77192129629629624</v>
       </c>
     </row>
-    <row r="389" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="389" spans="3:28">
       <c r="D389">
         <v>97</v>
       </c>
@@ -30791,9 +30783,9 @@
         <v>0.77195601851851858</v>
       </c>
     </row>
-    <row r="390" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="390" spans="3:28">
       <c r="C390" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D390">
         <v>98</v>
@@ -30871,7 +30863,7 @@
         <v>0.77249999999999996</v>
       </c>
     </row>
-    <row r="391" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="391" spans="3:28">
       <c r="D391">
         <v>98</v>
       </c>
@@ -30948,7 +30940,7 @@
         <v>0.77252314814814815</v>
       </c>
     </row>
-    <row r="392" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="392" spans="3:28">
       <c r="D392">
         <v>98</v>
       </c>
@@ -31025,7 +31017,7 @@
         <v>0.77254629629629623</v>
       </c>
     </row>
-    <row r="393" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="393" spans="3:28">
       <c r="D393">
         <v>98</v>
       </c>
@@ -31102,9 +31094,9 @@
         <v>0.77258101851851846</v>
       </c>
     </row>
-    <row r="394" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="394" spans="3:28">
       <c r="C394" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D394">
         <v>99</v>
@@ -31182,7 +31174,7 @@
         <v>0.77293981481481477</v>
       </c>
     </row>
-    <row r="395" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="395" spans="3:28">
       <c r="D395">
         <v>99</v>
       </c>
@@ -31259,7 +31251,7 @@
         <v>0.77296296296296296</v>
       </c>
     </row>
-    <row r="396" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="396" spans="3:28">
       <c r="D396">
         <v>99</v>
       </c>
@@ -31336,7 +31328,7 @@
         <v>0.77299768518518519</v>
       </c>
     </row>
-    <row r="397" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="397" spans="3:28">
       <c r="D397">
         <v>99</v>
       </c>
@@ -31413,9 +31405,9 @@
         <v>0.77303240740740742</v>
       </c>
     </row>
-    <row r="398" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="398" spans="3:28">
       <c r="C398" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D398">
         <v>100</v>
@@ -31493,7 +31485,7 @@
         <v>0.77474537037037028</v>
       </c>
     </row>
-    <row r="399" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="399" spans="3:28">
       <c r="D399">
         <v>100</v>
       </c>
@@ -31570,7 +31562,7 @@
         <v>0.77476851851851858</v>
       </c>
     </row>
-    <row r="400" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="400" spans="3:28">
       <c r="D400">
         <v>100</v>
       </c>
@@ -31647,7 +31639,7 @@
         <v>0.77483796296296292</v>
       </c>
     </row>
-    <row r="401" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="401" spans="3:28">
       <c r="D401">
         <v>100</v>
       </c>
@@ -31724,9 +31716,9 @@
         <v>0.77489583333333334</v>
       </c>
     </row>
-    <row r="402" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="402" spans="3:28">
       <c r="C402" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D402">
         <v>101</v>
@@ -31804,7 +31796,7 @@
         <v>0.77567129629629628</v>
       </c>
     </row>
-    <row r="403" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="403" spans="3:28">
       <c r="D403">
         <v>101</v>
       </c>
@@ -31881,7 +31873,7 @@
         <v>0.77572916666666669</v>
       </c>
     </row>
-    <row r="404" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="404" spans="3:28">
       <c r="D404">
         <v>101</v>
       </c>
@@ -31958,7 +31950,7 @@
         <v>0.77575231481481488</v>
       </c>
     </row>
-    <row r="405" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="405" spans="3:28">
       <c r="D405">
         <v>101</v>
       </c>

</xml_diff>